<commit_message>
add convert json to excel
</commit_message>
<xml_diff>
--- a/public/import/importExcelChance/data.xlsx
+++ b/public/import/importExcelChance/data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27960" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27960" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="A1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="4" r:id="rId2"/>
+    <sheet name="Arkusz3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>phone</t>
   </si>
@@ -399,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -479,12 +479,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="228">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>505505505</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="228">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>606606606</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="228">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>707707707</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -493,7 +547,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>

</xml_diff>